<commit_message>
modif url extension practitionerrole c191fca638fc3816e369783b688f9ba6c3151d9b
</commit_message>
<xml_diff>
--- a/sd-add-new-version-annuaire/ig/StructureDefinition-ror-location.xlsx
+++ b/sd-add-new-version-annuaire/ig/StructureDefinition-ror-location.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AM$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AM$134</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4776" uniqueCount="756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4742" uniqueCount="749">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-10T08:24:05+00:00</t>
+    <t>2024-04-10T09:05:12+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1852,10 +1852,6 @@
     <t>Location.address.line.extension.value[x]</t>
   </si>
   <si>
-    <t>base64Binary
-booleancanonicalcodedatedateTimedecimalidinstantintegermarkdownoidpositiveIntstringtimeunsignedInturiurluuidAddressAgeAnnotationAttachmentCodeableConceptCodingContactPointCountDistanceDurationHumanNameIdentifierMoneyPeriodQuantityRangeRatioReferenceSampledDataSignatureTimingContactDetailContributorDataRequirementExpressionParameterDefinitionRelatedArtifactTriggerDefinitionUsageContextDosageMeta</t>
-  </si>
-  <si>
     <t>Value of extension</t>
   </si>
   <si>
@@ -1865,26 +1861,7 @@
     <t>https://mos.esante.gouv.fr/NOS/JDV_J219-TypeVoie-ROR/FHIR/JDV-J219-TypeVoie-ROR</t>
   </si>
   <si>
-    <t xml:space="preserve">type:$this}
-</t>
-  </si>
-  <si>
-    <t>closed</t>
-  </si>
-  <si>
     <t>Extension.value[x]</t>
-  </si>
-  <si>
-    <t>Location.address.line.extension:streetNameType.value[x]:valueString</t>
-  </si>
-  <si>
-    <t>valueString</t>
-  </si>
-  <si>
-    <t>JDV_J103-TypeVoie-RASS</t>
-  </si>
-  <si>
-    <t>https://mos.esante.gouv.fr/NOS/JDV_J103-TypeVoie-RASS/FHIR/JDV-J103-TypeVoie-RASS</t>
   </si>
   <si>
     <t>Location.address.line.extension:streetNameBase</t>
@@ -1944,7 +1921,7 @@
     <t>lieuDit (Adresse) : Lieu qui porte un nom rappelant une particularité topographique ou historique</t>
   </si>
   <si>
-    <t>Extension créée dans le cadre du ROR pour indiquer le lieu dit</t>
+    <t>Extension créée dans le cadre de l'Annuaire Santé pour indiquer le lieu dit</t>
   </si>
   <si>
     <t>Location.address.line.value</t>
@@ -2675,7 +2652,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM135"/>
+  <dimension ref="A1:AM134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -2684,7 +2661,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="65.2265625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="60.4296875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="42.98046875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="34.48828125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
@@ -2694,7 +2671,7 @@
     <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="255.0" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="138.9140625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -13874,7 +13851,7 @@
         <v>76</v>
       </c>
       <c r="G101" t="s" s="2">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H101" t="s" s="2">
         <v>75</v>
@@ -14093,7 +14070,7 @@
       </c>
       <c r="E103" s="2"/>
       <c r="F103" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="G103" t="s" s="2">
         <v>85</v>
@@ -14108,13 +14085,13 @@
         <v>75</v>
       </c>
       <c r="K103" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="L103" t="s" s="2">
         <v>594</v>
       </c>
-      <c r="L103" t="s" s="2">
+      <c r="M103" t="s" s="2">
         <v>595</v>
-      </c>
-      <c r="M103" t="s" s="2">
-        <v>596</v>
       </c>
       <c r="N103" s="2"/>
       <c r="O103" s="2"/>
@@ -14145,23 +14122,25 @@
       </c>
       <c r="Y103" s="2"/>
       <c r="Z103" t="s" s="2">
+        <v>596</v>
+      </c>
+      <c r="AA103" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB103" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC103" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD103" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE103" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF103" t="s" s="2">
         <v>597</v>
-      </c>
-      <c r="AA103" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AB103" t="s" s="2">
-        <v>598</v>
-      </c>
-      <c r="AC103" s="2"/>
-      <c r="AD103" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AE103" t="s" s="2">
-        <v>599</v>
-      </c>
-      <c r="AF103" t="s" s="2">
-        <v>600</v>
       </c>
       <c r="AG103" t="s" s="2">
         <v>76</v>
@@ -14187,13 +14166,13 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="B104" t="s" s="2">
-        <v>593</v>
+        <v>545</v>
       </c>
       <c r="C104" t="s" s="2">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D104" t="s" s="2">
         <v>75</v>
@@ -14206,7 +14185,7 @@
         <v>85</v>
       </c>
       <c r="H104" t="s" s="2">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="I104" t="s" s="2">
         <v>75</v>
@@ -14215,13 +14194,13 @@
         <v>75</v>
       </c>
       <c r="K104" t="s" s="2">
-        <v>103</v>
+        <v>600</v>
       </c>
       <c r="L104" t="s" s="2">
-        <v>595</v>
+        <v>601</v>
       </c>
       <c r="M104" t="s" s="2">
-        <v>596</v>
+        <v>602</v>
       </c>
       <c r="N104" s="2"/>
       <c r="O104" s="2"/>
@@ -14248,13 +14227,13 @@
         <v>75</v>
       </c>
       <c r="X104" t="s" s="2">
-        <v>164</v>
+        <v>75</v>
       </c>
       <c r="Y104" t="s" s="2">
-        <v>603</v>
+        <v>75</v>
       </c>
       <c r="Z104" t="s" s="2">
-        <v>604</v>
+        <v>75</v>
       </c>
       <c r="AA104" t="s" s="2">
         <v>75</v>
@@ -14272,25 +14251,25 @@
         <v>75</v>
       </c>
       <c r="AF104" t="s" s="2">
-        <v>600</v>
+        <v>117</v>
       </c>
       <c r="AG104" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH104" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AI104" t="s" s="2">
         <v>98</v>
       </c>
       <c r="AJ104" t="s" s="2">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="AK104" t="s" s="2">
-        <v>75</v>
+        <v>603</v>
       </c>
       <c r="AL104" t="s" s="2">
-        <v>101</v>
+        <v>604</v>
       </c>
       <c r="AM104" t="s" s="2">
         <v>75</v>
@@ -14509,10 +14488,10 @@
         <v>118</v>
       </c>
       <c r="AK106" t="s" s="2">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="AL106" t="s" s="2">
-        <v>618</v>
+        <v>75</v>
       </c>
       <c r="AM106" t="s" s="2">
         <v>75</v>
@@ -14520,14 +14499,12 @@
     </row>
     <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B107" t="s" s="2">
-        <v>545</v>
-      </c>
-      <c r="C107" t="s" s="2">
-        <v>620</v>
-      </c>
+        <v>617</v>
+      </c>
+      <c r="C107" s="2"/>
       <c r="D107" t="s" s="2">
         <v>75</v>
       </c>
@@ -14539,7 +14516,7 @@
         <v>85</v>
       </c>
       <c r="H107" t="s" s="2">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="I107" t="s" s="2">
         <v>75</v>
@@ -14548,13 +14525,13 @@
         <v>75</v>
       </c>
       <c r="K107" t="s" s="2">
-        <v>621</v>
+        <v>103</v>
       </c>
       <c r="L107" t="s" s="2">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="M107" t="s" s="2">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="N107" s="2"/>
       <c r="O107" s="2"/>
@@ -14578,7 +14555,7 @@
         <v>75</v>
       </c>
       <c r="W107" t="s" s="2">
-        <v>75</v>
+        <v>619</v>
       </c>
       <c r="X107" t="s" s="2">
         <v>75</v>
@@ -14605,22 +14582,22 @@
         <v>75</v>
       </c>
       <c r="AF107" t="s" s="2">
-        <v>117</v>
+        <v>620</v>
       </c>
       <c r="AG107" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH107" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="AI107" t="s" s="2">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="AJ107" t="s" s="2">
-        <v>118</v>
+        <v>75</v>
       </c>
       <c r="AK107" t="s" s="2">
-        <v>620</v>
+        <v>75</v>
       </c>
       <c r="AL107" t="s" s="2">
         <v>75</v>
@@ -14631,14 +14608,14 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="B108" t="s" s="2">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" t="s" s="2">
-        <v>75</v>
+        <v>622</v>
       </c>
       <c r="E108" s="2"/>
       <c r="F108" t="s" s="2">
@@ -14654,18 +14631,20 @@
         <v>75</v>
       </c>
       <c r="J108" t="s" s="2">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="K108" t="s" s="2">
         <v>103</v>
       </c>
       <c r="L108" t="s" s="2">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="M108" t="s" s="2">
-        <v>625</v>
-      </c>
-      <c r="N108" s="2"/>
+        <v>624</v>
+      </c>
+      <c r="N108" t="s" s="2">
+        <v>306</v>
+      </c>
       <c r="O108" s="2"/>
       <c r="P108" t="s" s="2">
         <v>75</v>
@@ -14678,7 +14657,7 @@
         <v>75</v>
       </c>
       <c r="T108" t="s" s="2">
-        <v>75</v>
+        <v>625</v>
       </c>
       <c r="U108" t="s" s="2">
         <v>75</v>
@@ -14687,52 +14666,52 @@
         <v>75</v>
       </c>
       <c r="W108" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X108" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y108" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z108" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA108" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB108" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC108" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD108" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE108" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF108" t="s" s="2">
         <v>626</v>
       </c>
-      <c r="X108" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="Y108" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="Z108" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AA108" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AB108" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AC108" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AD108" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AE108" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AF108" t="s" s="2">
+      <c r="AG108" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH108" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="AI108" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="AJ108" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AK108" t="s" s="2">
         <v>627</v>
       </c>
-      <c r="AG108" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AH108" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="AI108" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AJ108" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AK108" t="s" s="2">
-        <v>75</v>
-      </c>
       <c r="AL108" t="s" s="2">
-        <v>75</v>
+        <v>628</v>
       </c>
       <c r="AM108" t="s" s="2">
         <v>75</v>
@@ -14740,14 +14719,14 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B109" t="s" s="2">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" t="s" s="2">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="E109" s="2"/>
       <c r="F109" t="s" s="2">
@@ -14769,13 +14748,13 @@
         <v>103</v>
       </c>
       <c r="L109" t="s" s="2">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="M109" t="s" s="2">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="N109" t="s" s="2">
-        <v>306</v>
+        <v>633</v>
       </c>
       <c r="O109" s="2"/>
       <c r="P109" t="s" s="2">
@@ -14789,7 +14768,7 @@
         <v>75</v>
       </c>
       <c r="T109" t="s" s="2">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="U109" t="s" s="2">
         <v>75</v>
@@ -14825,7 +14804,7 @@
         <v>75</v>
       </c>
       <c r="AF109" t="s" s="2">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="AG109" t="s" s="2">
         <v>76</v>
@@ -14840,10 +14819,10 @@
         <v>99</v>
       </c>
       <c r="AK109" t="s" s="2">
-        <v>634</v>
+        <v>75</v>
       </c>
       <c r="AL109" t="s" s="2">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="AM109" t="s" s="2">
         <v>75</v>
@@ -14851,14 +14830,14 @@
     </row>
     <row r="110" hidden="true">
       <c r="A110" t="s" s="2">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="B110" t="s" s="2">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="C110" s="2"/>
       <c r="D110" t="s" s="2">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="E110" s="2"/>
       <c r="F110" t="s" s="2">
@@ -14880,13 +14859,13 @@
         <v>103</v>
       </c>
       <c r="L110" t="s" s="2">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="M110" t="s" s="2">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="N110" t="s" s="2">
-        <v>640</v>
+        <v>306</v>
       </c>
       <c r="O110" s="2"/>
       <c r="P110" t="s" s="2">
@@ -14900,43 +14879,43 @@
         <v>75</v>
       </c>
       <c r="T110" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U110" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V110" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W110" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X110" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y110" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z110" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA110" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB110" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC110" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD110" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE110" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF110" t="s" s="2">
         <v>641</v>
-      </c>
-      <c r="U110" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="V110" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="W110" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="X110" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="Y110" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="Z110" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AA110" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AB110" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AC110" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AD110" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AE110" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AF110" t="s" s="2">
-        <v>642</v>
       </c>
       <c r="AG110" t="s" s="2">
         <v>76</v>
@@ -14954,7 +14933,7 @@
         <v>75</v>
       </c>
       <c r="AL110" t="s" s="2">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AM110" t="s" s="2">
         <v>75</v>
@@ -14962,14 +14941,14 @@
     </row>
     <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B111" t="s" s="2">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" t="s" s="2">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E111" s="2"/>
       <c r="F111" t="s" s="2">
@@ -14991,10 +14970,10 @@
         <v>103</v>
       </c>
       <c r="L111" t="s" s="2">
+        <v>645</v>
+      </c>
+      <c r="M111" t="s" s="2">
         <v>646</v>
-      </c>
-      <c r="M111" t="s" s="2">
-        <v>647</v>
       </c>
       <c r="N111" t="s" s="2">
         <v>306</v>
@@ -15011,7 +14990,7 @@
         <v>75</v>
       </c>
       <c r="T111" t="s" s="2">
-        <v>75</v>
+        <v>647</v>
       </c>
       <c r="U111" t="s" s="2">
         <v>75</v>
@@ -15062,10 +15041,10 @@
         <v>99</v>
       </c>
       <c r="AK111" t="s" s="2">
-        <v>75</v>
+        <v>649</v>
       </c>
       <c r="AL111" t="s" s="2">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="AM111" t="s" s="2">
         <v>75</v>
@@ -15073,14 +15052,14 @@
     </row>
     <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B112" t="s" s="2">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" t="s" s="2">
-        <v>651</v>
+        <v>75</v>
       </c>
       <c r="E112" s="2"/>
       <c r="F112" t="s" s="2">
@@ -15108,7 +15087,7 @@
         <v>653</v>
       </c>
       <c r="N112" t="s" s="2">
-        <v>306</v>
+        <v>654</v>
       </c>
       <c r="O112" s="2"/>
       <c r="P112" t="s" s="2">
@@ -15122,7 +15101,7 @@
         <v>75</v>
       </c>
       <c r="T112" t="s" s="2">
-        <v>654</v>
+        <v>75</v>
       </c>
       <c r="U112" t="s" s="2">
         <v>75</v>
@@ -15173,10 +15152,10 @@
         <v>99</v>
       </c>
       <c r="AK112" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL112" t="s" s="2">
         <v>656</v>
-      </c>
-      <c r="AL112" t="s" s="2">
-        <v>657</v>
       </c>
       <c r="AM112" t="s" s="2">
         <v>75</v>
@@ -15184,10 +15163,10 @@
     </row>
     <row r="113" hidden="true">
       <c r="A113" t="s" s="2">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B113" t="s" s="2">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" t="s" s="2">
@@ -15210,18 +15189,20 @@
         <v>86</v>
       </c>
       <c r="K113" t="s" s="2">
-        <v>103</v>
+        <v>354</v>
       </c>
       <c r="L113" t="s" s="2">
+        <v>658</v>
+      </c>
+      <c r="M113" t="s" s="2">
         <v>659</v>
       </c>
-      <c r="M113" t="s" s="2">
+      <c r="N113" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="O113" t="s" s="2">
         <v>660</v>
       </c>
-      <c r="N113" t="s" s="2">
-        <v>661</v>
-      </c>
-      <c r="O113" s="2"/>
       <c r="P113" t="s" s="2">
         <v>75</v>
       </c>
@@ -15233,7 +15214,7 @@
         <v>75</v>
       </c>
       <c r="T113" t="s" s="2">
-        <v>75</v>
+        <v>661</v>
       </c>
       <c r="U113" t="s" s="2">
         <v>75</v>
@@ -15281,13 +15262,13 @@
         <v>98</v>
       </c>
       <c r="AJ113" t="s" s="2">
-        <v>99</v>
+        <v>359</v>
       </c>
       <c r="AK113" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AL113" t="s" s="2">
-        <v>663</v>
+        <v>502</v>
       </c>
       <c r="AM113" t="s" s="2">
         <v>75</v>
@@ -15295,10 +15276,10 @@
     </row>
     <row r="114" hidden="true">
       <c r="A114" t="s" s="2">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B114" t="s" s="2">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" t="s" s="2">
@@ -15321,19 +15302,19 @@
         <v>86</v>
       </c>
       <c r="K114" t="s" s="2">
-        <v>354</v>
+        <v>263</v>
       </c>
       <c r="L114" t="s" s="2">
+        <v>664</v>
+      </c>
+      <c r="M114" t="s" s="2">
         <v>665</v>
       </c>
-      <c r="M114" t="s" s="2">
+      <c r="N114" t="s" s="2">
+        <v>439</v>
+      </c>
+      <c r="O114" t="s" s="2">
         <v>666</v>
-      </c>
-      <c r="N114" t="s" s="2">
-        <v>357</v>
-      </c>
-      <c r="O114" t="s" s="2">
-        <v>667</v>
       </c>
       <c r="P114" t="s" s="2">
         <v>75</v>
@@ -15346,26 +15327,26 @@
         <v>75</v>
       </c>
       <c r="T114" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U114" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V114" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W114" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X114" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="Y114" t="s" s="2">
+        <v>667</v>
+      </c>
+      <c r="Z114" t="s" s="2">
         <v>668</v>
       </c>
-      <c r="U114" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="V114" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="W114" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="X114" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="Y114" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="Z114" t="s" s="2">
-        <v>75</v>
-      </c>
       <c r="AA114" t="s" s="2">
         <v>75</v>
       </c>
@@ -15382,7 +15363,7 @@
         <v>75</v>
       </c>
       <c r="AF114" t="s" s="2">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="AG114" t="s" s="2">
         <v>76</v>
@@ -15394,16 +15375,16 @@
         <v>98</v>
       </c>
       <c r="AJ114" t="s" s="2">
-        <v>359</v>
+        <v>99</v>
       </c>
       <c r="AK114" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AL114" t="s" s="2">
-        <v>502</v>
+        <v>669</v>
       </c>
       <c r="AM114" t="s" s="2">
-        <v>75</v>
+        <v>435</v>
       </c>
     </row>
     <row r="115" hidden="true">
@@ -15431,22 +15412,20 @@
         <v>75</v>
       </c>
       <c r="J115" t="s" s="2">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K115" t="s" s="2">
-        <v>263</v>
+        <v>671</v>
       </c>
       <c r="L115" t="s" s="2">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="M115" t="s" s="2">
-        <v>672</v>
-      </c>
-      <c r="N115" t="s" s="2">
-        <v>439</v>
-      </c>
+        <v>673</v>
+      </c>
+      <c r="N115" s="2"/>
       <c r="O115" t="s" s="2">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="P115" t="s" s="2">
         <v>75</v>
@@ -15471,13 +15450,13 @@
         <v>75</v>
       </c>
       <c r="X115" t="s" s="2">
-        <v>157</v>
+        <v>75</v>
       </c>
       <c r="Y115" t="s" s="2">
-        <v>674</v>
+        <v>75</v>
       </c>
       <c r="Z115" t="s" s="2">
-        <v>675</v>
+        <v>75</v>
       </c>
       <c r="AA115" t="s" s="2">
         <v>75</v>
@@ -15510,13 +15489,13 @@
         <v>99</v>
       </c>
       <c r="AK115" t="s" s="2">
-        <v>75</v>
+        <v>675</v>
       </c>
       <c r="AL115" t="s" s="2">
         <v>676</v>
       </c>
       <c r="AM115" t="s" s="2">
-        <v>435</v>
+        <v>75</v>
       </c>
     </row>
     <row r="116" hidden="true">
@@ -15547,18 +15526,16 @@
         <v>75</v>
       </c>
       <c r="K116" t="s" s="2">
-        <v>678</v>
+        <v>103</v>
       </c>
       <c r="L116" t="s" s="2">
-        <v>679</v>
+        <v>104</v>
       </c>
       <c r="M116" t="s" s="2">
-        <v>680</v>
+        <v>105</v>
       </c>
       <c r="N116" s="2"/>
-      <c r="O116" t="s" s="2">
-        <v>681</v>
-      </c>
+      <c r="O116" s="2"/>
       <c r="P116" t="s" s="2">
         <v>75</v>
       </c>
@@ -15606,7 +15583,7 @@
         <v>75</v>
       </c>
       <c r="AF116" t="s" s="2">
-        <v>677</v>
+        <v>106</v>
       </c>
       <c r="AG116" t="s" s="2">
         <v>76</v>
@@ -15615,16 +15592,16 @@
         <v>85</v>
       </c>
       <c r="AI116" t="s" s="2">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="AJ116" t="s" s="2">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="AK116" t="s" s="2">
-        <v>682</v>
+        <v>75</v>
       </c>
       <c r="AL116" t="s" s="2">
-        <v>683</v>
+        <v>107</v>
       </c>
       <c r="AM116" t="s" s="2">
         <v>75</v>
@@ -15632,21 +15609,21 @@
     </row>
     <row r="117" hidden="true">
       <c r="A117" t="s" s="2">
-        <v>684</v>
+        <v>678</v>
       </c>
       <c r="B117" t="s" s="2">
-        <v>684</v>
+        <v>678</v>
       </c>
       <c r="C117" s="2"/>
       <c r="D117" t="s" s="2">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="E117" s="2"/>
       <c r="F117" t="s" s="2">
         <v>76</v>
       </c>
       <c r="G117" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H117" t="s" s="2">
         <v>75</v>
@@ -15658,15 +15635,17 @@
         <v>75</v>
       </c>
       <c r="K117" t="s" s="2">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="L117" t="s" s="2">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="M117" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="N117" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="N117" t="s" s="2">
+        <v>113</v>
+      </c>
       <c r="O117" s="2"/>
       <c r="P117" t="s" s="2">
         <v>75</v>
@@ -15703,37 +15682,37 @@
         <v>75</v>
       </c>
       <c r="AB117" t="s" s="2">
-        <v>75</v>
+        <v>114</v>
       </c>
       <c r="AC117" t="s" s="2">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="AD117" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AE117" t="s" s="2">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="AF117" t="s" s="2">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="AG117" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH117" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AI117" t="s" s="2">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="AJ117" t="s" s="2">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="AK117" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AL117" t="s" s="2">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AM117" t="s" s="2">
         <v>75</v>
@@ -15741,24 +15720,26 @@
     </row>
     <row r="118" hidden="true">
       <c r="A118" t="s" s="2">
-        <v>685</v>
+        <v>679</v>
       </c>
       <c r="B118" t="s" s="2">
-        <v>685</v>
-      </c>
-      <c r="C118" s="2"/>
+        <v>678</v>
+      </c>
+      <c r="C118" t="s" s="2">
+        <v>680</v>
+      </c>
       <c r="D118" t="s" s="2">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="E118" s="2"/>
       <c r="F118" t="s" s="2">
         <v>76</v>
       </c>
       <c r="G118" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H118" t="s" s="2">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="I118" t="s" s="2">
         <v>75</v>
@@ -15767,17 +15748,15 @@
         <v>75</v>
       </c>
       <c r="K118" t="s" s="2">
-        <v>110</v>
+        <v>681</v>
       </c>
       <c r="L118" t="s" s="2">
-        <v>111</v>
+        <v>682</v>
       </c>
       <c r="M118" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="N118" t="s" s="2">
-        <v>113</v>
-      </c>
+        <v>683</v>
+      </c>
+      <c r="N118" s="2"/>
       <c r="O118" s="2"/>
       <c r="P118" t="s" s="2">
         <v>75</v>
@@ -15814,16 +15793,16 @@
         <v>75</v>
       </c>
       <c r="AB118" t="s" s="2">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="AC118" t="s" s="2">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="AD118" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AE118" t="s" s="2">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="AF118" t="s" s="2">
         <v>117</v>
@@ -15844,7 +15823,7 @@
         <v>75</v>
       </c>
       <c r="AL118" t="s" s="2">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="AM118" t="s" s="2">
         <v>75</v>
@@ -15852,44 +15831,46 @@
     </row>
     <row r="119" hidden="true">
       <c r="A119" t="s" s="2">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B119" t="s" s="2">
+        <v>684</v>
+      </c>
+      <c r="C119" s="2"/>
+      <c r="D119" t="s" s="2">
         <v>685</v>
-      </c>
-      <c r="C119" t="s" s="2">
-        <v>687</v>
-      </c>
-      <c r="D119" t="s" s="2">
-        <v>75</v>
       </c>
       <c r="E119" s="2"/>
       <c r="F119" t="s" s="2">
         <v>76</v>
       </c>
       <c r="G119" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H119" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I119" t="s" s="2">
         <v>86</v>
       </c>
-      <c r="I119" t="s" s="2">
-        <v>75</v>
-      </c>
       <c r="J119" t="s" s="2">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="K119" t="s" s="2">
-        <v>688</v>
+        <v>110</v>
       </c>
       <c r="L119" t="s" s="2">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="M119" t="s" s="2">
-        <v>690</v>
-      </c>
-      <c r="N119" s="2"/>
-      <c r="O119" s="2"/>
+        <v>687</v>
+      </c>
+      <c r="N119" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="O119" t="s" s="2">
+        <v>234</v>
+      </c>
       <c r="P119" t="s" s="2">
         <v>75</v>
       </c>
@@ -15937,7 +15918,7 @@
         <v>75</v>
       </c>
       <c r="AF119" t="s" s="2">
-        <v>117</v>
+        <v>688</v>
       </c>
       <c r="AG119" t="s" s="2">
         <v>76</v>
@@ -15955,7 +15936,7 @@
         <v>75</v>
       </c>
       <c r="AL119" t="s" s="2">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="AM119" t="s" s="2">
         <v>75</v>
@@ -15963,46 +15944,44 @@
     </row>
     <row r="120" hidden="true">
       <c r="A120" t="s" s="2">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B120" t="s" s="2">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="C120" s="2"/>
       <c r="D120" t="s" s="2">
-        <v>692</v>
+        <v>75</v>
       </c>
       <c r="E120" s="2"/>
       <c r="F120" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="G120" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H120" t="s" s="2">
         <v>75</v>
       </c>
       <c r="I120" t="s" s="2">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="J120" t="s" s="2">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K120" t="s" s="2">
-        <v>110</v>
+        <v>690</v>
       </c>
       <c r="L120" t="s" s="2">
+        <v>691</v>
+      </c>
+      <c r="M120" t="s" s="2">
+        <v>692</v>
+      </c>
+      <c r="N120" t="s" s="2">
         <v>693</v>
       </c>
-      <c r="M120" t="s" s="2">
-        <v>694</v>
-      </c>
-      <c r="N120" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="O120" t="s" s="2">
-        <v>234</v>
-      </c>
+      <c r="O120" s="2"/>
       <c r="P120" t="s" s="2">
         <v>75</v>
       </c>
@@ -16050,25 +16029,25 @@
         <v>75</v>
       </c>
       <c r="AF120" t="s" s="2">
-        <v>695</v>
+        <v>689</v>
       </c>
       <c r="AG120" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="AH120" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="AI120" t="s" s="2">
         <v>98</v>
       </c>
       <c r="AJ120" t="s" s="2">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="AK120" t="s" s="2">
-        <v>75</v>
+        <v>694</v>
       </c>
       <c r="AL120" t="s" s="2">
-        <v>101</v>
+        <v>695</v>
       </c>
       <c r="AM120" t="s" s="2">
         <v>75</v>
@@ -16102,16 +16081,16 @@
         <v>75</v>
       </c>
       <c r="K121" t="s" s="2">
+        <v>690</v>
+      </c>
+      <c r="L121" t="s" s="2">
         <v>697</v>
       </c>
-      <c r="L121" t="s" s="2">
+      <c r="M121" t="s" s="2">
         <v>698</v>
       </c>
-      <c r="M121" t="s" s="2">
-        <v>699</v>
-      </c>
       <c r="N121" t="s" s="2">
-        <v>700</v>
+        <v>693</v>
       </c>
       <c r="O121" s="2"/>
       <c r="P121" t="s" s="2">
@@ -16176,10 +16155,10 @@
         <v>99</v>
       </c>
       <c r="AK121" t="s" s="2">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="AL121" t="s" s="2">
-        <v>702</v>
+        <v>695</v>
       </c>
       <c r="AM121" t="s" s="2">
         <v>75</v>
@@ -16187,10 +16166,10 @@
     </row>
     <row r="122" hidden="true">
       <c r="A122" t="s" s="2">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="B122" t="s" s="2">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="C122" s="2"/>
       <c r="D122" t="s" s="2">
@@ -16198,7 +16177,7 @@
       </c>
       <c r="E122" s="2"/>
       <c r="F122" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G122" t="s" s="2">
         <v>85</v>
@@ -16213,16 +16192,16 @@
         <v>75</v>
       </c>
       <c r="K122" t="s" s="2">
-        <v>697</v>
+        <v>690</v>
       </c>
       <c r="L122" t="s" s="2">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="M122" t="s" s="2">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="N122" t="s" s="2">
-        <v>700</v>
+        <v>693</v>
       </c>
       <c r="O122" s="2"/>
       <c r="P122" t="s" s="2">
@@ -16272,10 +16251,10 @@
         <v>75</v>
       </c>
       <c r="AF122" t="s" s="2">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="AG122" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AH122" t="s" s="2">
         <v>85</v>
@@ -16287,10 +16266,10 @@
         <v>99</v>
       </c>
       <c r="AK122" t="s" s="2">
-        <v>706</v>
+        <v>75</v>
       </c>
       <c r="AL122" t="s" s="2">
-        <v>702</v>
+        <v>695</v>
       </c>
       <c r="AM122" t="s" s="2">
         <v>75</v>
@@ -16298,10 +16277,10 @@
     </row>
     <row r="123" hidden="true">
       <c r="A123" t="s" s="2">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="B123" t="s" s="2">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="C123" s="2"/>
       <c r="D123" t="s" s="2">
@@ -16315,27 +16294,29 @@
         <v>85</v>
       </c>
       <c r="H123" t="s" s="2">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="I123" t="s" s="2">
         <v>75</v>
       </c>
       <c r="J123" t="s" s="2">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="K123" t="s" s="2">
-        <v>697</v>
+        <v>704</v>
       </c>
       <c r="L123" t="s" s="2">
+        <v>705</v>
+      </c>
+      <c r="M123" t="s" s="2">
+        <v>706</v>
+      </c>
+      <c r="N123" t="s" s="2">
+        <v>707</v>
+      </c>
+      <c r="O123" t="s" s="2">
         <v>708</v>
       </c>
-      <c r="M123" t="s" s="2">
-        <v>709</v>
-      </c>
-      <c r="N123" t="s" s="2">
-        <v>700</v>
-      </c>
-      <c r="O123" s="2"/>
       <c r="P123" t="s" s="2">
         <v>75</v>
       </c>
@@ -16383,7 +16364,7 @@
         <v>75</v>
       </c>
       <c r="AF123" t="s" s="2">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="AG123" t="s" s="2">
         <v>76</v>
@@ -16395,13 +16376,13 @@
         <v>98</v>
       </c>
       <c r="AJ123" t="s" s="2">
-        <v>99</v>
+        <v>368</v>
       </c>
       <c r="AK123" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AL123" t="s" s="2">
-        <v>702</v>
+        <v>709</v>
       </c>
       <c r="AM123" t="s" s="2">
         <v>75</v>
@@ -16426,13 +16407,13 @@
         <v>85</v>
       </c>
       <c r="H124" t="s" s="2">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="I124" t="s" s="2">
         <v>75</v>
       </c>
       <c r="J124" t="s" s="2">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K124" t="s" s="2">
         <v>711</v>
@@ -16536,7 +16517,7 @@
         <v>76</v>
       </c>
       <c r="G125" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H125" t="s" s="2">
         <v>75</v>
@@ -16548,20 +16529,18 @@
         <v>75</v>
       </c>
       <c r="K125" t="s" s="2">
+        <v>671</v>
+      </c>
+      <c r="L125" t="s" s="2">
         <v>718</v>
       </c>
-      <c r="L125" t="s" s="2">
+      <c r="M125" t="s" s="2">
         <v>719</v>
       </c>
-      <c r="M125" t="s" s="2">
+      <c r="N125" t="s" s="2">
         <v>720</v>
       </c>
-      <c r="N125" t="s" s="2">
-        <v>721</v>
-      </c>
-      <c r="O125" t="s" s="2">
-        <v>722</v>
-      </c>
+      <c r="O125" s="2"/>
       <c r="P125" t="s" s="2">
         <v>75</v>
       </c>
@@ -16615,19 +16594,19 @@
         <v>76</v>
       </c>
       <c r="AH125" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AI125" t="s" s="2">
         <v>98</v>
       </c>
       <c r="AJ125" t="s" s="2">
-        <v>368</v>
+        <v>99</v>
       </c>
       <c r="AK125" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AL125" t="s" s="2">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="AM125" t="s" s="2">
         <v>75</v>
@@ -16635,10 +16614,10 @@
     </row>
     <row r="126" hidden="true">
       <c r="A126" t="s" s="2">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B126" t="s" s="2">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="C126" s="2"/>
       <c r="D126" t="s" s="2">
@@ -16649,7 +16628,7 @@
         <v>76</v>
       </c>
       <c r="G126" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H126" t="s" s="2">
         <v>75</v>
@@ -16661,17 +16640,15 @@
         <v>75</v>
       </c>
       <c r="K126" t="s" s="2">
-        <v>678</v>
+        <v>103</v>
       </c>
       <c r="L126" t="s" s="2">
-        <v>725</v>
+        <v>104</v>
       </c>
       <c r="M126" t="s" s="2">
-        <v>726</v>
-      </c>
-      <c r="N126" t="s" s="2">
-        <v>727</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="N126" s="2"/>
       <c r="O126" s="2"/>
       <c r="P126" t="s" s="2">
         <v>75</v>
@@ -16720,25 +16697,25 @@
         <v>75</v>
       </c>
       <c r="AF126" t="s" s="2">
-        <v>724</v>
+        <v>106</v>
       </c>
       <c r="AG126" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH126" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="AI126" t="s" s="2">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="AJ126" t="s" s="2">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="AK126" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AL126" t="s" s="2">
-        <v>728</v>
+        <v>107</v>
       </c>
       <c r="AM126" t="s" s="2">
         <v>75</v>
@@ -16746,21 +16723,21 @@
     </row>
     <row r="127" hidden="true">
       <c r="A127" t="s" s="2">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="B127" t="s" s="2">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="C127" s="2"/>
       <c r="D127" t="s" s="2">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="E127" s="2"/>
       <c r="F127" t="s" s="2">
         <v>76</v>
       </c>
       <c r="G127" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H127" t="s" s="2">
         <v>75</v>
@@ -16772,15 +16749,17 @@
         <v>75</v>
       </c>
       <c r="K127" t="s" s="2">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="L127" t="s" s="2">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="M127" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="N127" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="N127" t="s" s="2">
+        <v>113</v>
+      </c>
       <c r="O127" s="2"/>
       <c r="P127" t="s" s="2">
         <v>75</v>
@@ -16817,37 +16796,37 @@
         <v>75</v>
       </c>
       <c r="AB127" t="s" s="2">
-        <v>75</v>
+        <v>114</v>
       </c>
       <c r="AC127" t="s" s="2">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="AD127" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AE127" t="s" s="2">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="AF127" t="s" s="2">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="AG127" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH127" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AI127" t="s" s="2">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="AJ127" t="s" s="2">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="AK127" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AL127" t="s" s="2">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AM127" t="s" s="2">
         <v>75</v>
@@ -16855,14 +16834,14 @@
     </row>
     <row r="128" hidden="true">
       <c r="A128" t="s" s="2">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="B128" t="s" s="2">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="C128" s="2"/>
       <c r="D128" t="s" s="2">
-        <v>109</v>
+        <v>685</v>
       </c>
       <c r="E128" s="2"/>
       <c r="F128" t="s" s="2">
@@ -16875,24 +16854,26 @@
         <v>75</v>
       </c>
       <c r="I128" t="s" s="2">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="J128" t="s" s="2">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="K128" t="s" s="2">
         <v>110</v>
       </c>
       <c r="L128" t="s" s="2">
-        <v>111</v>
+        <v>686</v>
       </c>
       <c r="M128" t="s" s="2">
-        <v>112</v>
+        <v>687</v>
       </c>
       <c r="N128" t="s" s="2">
         <v>113</v>
       </c>
-      <c r="O128" s="2"/>
+      <c r="O128" t="s" s="2">
+        <v>234</v>
+      </c>
       <c r="P128" t="s" s="2">
         <v>75</v>
       </c>
@@ -16928,19 +16909,19 @@
         <v>75</v>
       </c>
       <c r="AB128" t="s" s="2">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="AC128" t="s" s="2">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="AD128" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AE128" t="s" s="2">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="AF128" t="s" s="2">
-        <v>117</v>
+        <v>688</v>
       </c>
       <c r="AG128" t="s" s="2">
         <v>76</v>
@@ -16966,14 +16947,14 @@
     </row>
     <row r="129" hidden="true">
       <c r="A129" t="s" s="2">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="B129" t="s" s="2">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="C129" s="2"/>
       <c r="D129" t="s" s="2">
-        <v>692</v>
+        <v>75</v>
       </c>
       <c r="E129" s="2"/>
       <c r="F129" t="s" s="2">
@@ -16986,26 +16967,24 @@
         <v>75</v>
       </c>
       <c r="I129" t="s" s="2">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="J129" t="s" s="2">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K129" t="s" s="2">
-        <v>110</v>
+        <v>173</v>
       </c>
       <c r="L129" t="s" s="2">
-        <v>693</v>
+        <v>726</v>
       </c>
       <c r="M129" t="s" s="2">
-        <v>694</v>
+        <v>727</v>
       </c>
       <c r="N129" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="O129" t="s" s="2">
-        <v>234</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="O129" s="2"/>
       <c r="P129" t="s" s="2">
         <v>75</v>
       </c>
@@ -17029,13 +17008,13 @@
         <v>75</v>
       </c>
       <c r="X129" t="s" s="2">
-        <v>75</v>
+        <v>164</v>
       </c>
       <c r="Y129" t="s" s="2">
-        <v>75</v>
+        <v>728</v>
       </c>
       <c r="Z129" t="s" s="2">
-        <v>75</v>
+        <v>729</v>
       </c>
       <c r="AA129" t="s" s="2">
         <v>75</v>
@@ -17053,7 +17032,7 @@
         <v>75</v>
       </c>
       <c r="AF129" t="s" s="2">
-        <v>695</v>
+        <v>725</v>
       </c>
       <c r="AG129" t="s" s="2">
         <v>76</v>
@@ -17065,13 +17044,13 @@
         <v>98</v>
       </c>
       <c r="AJ129" t="s" s="2">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="AK129" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AL129" t="s" s="2">
-        <v>101</v>
+        <v>721</v>
       </c>
       <c r="AM129" t="s" s="2">
         <v>75</v>
@@ -17079,10 +17058,10 @@
     </row>
     <row r="130" hidden="true">
       <c r="A130" t="s" s="2">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B130" t="s" s="2">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C130" s="2"/>
       <c r="D130" t="s" s="2">
@@ -17093,7 +17072,7 @@
         <v>76</v>
       </c>
       <c r="G130" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H130" t="s" s="2">
         <v>75</v>
@@ -17105,17 +17084,15 @@
         <v>75</v>
       </c>
       <c r="K130" t="s" s="2">
-        <v>173</v>
+        <v>320</v>
       </c>
       <c r="L130" t="s" s="2">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="M130" t="s" s="2">
-        <v>734</v>
-      </c>
-      <c r="N130" t="s" s="2">
-        <v>306</v>
-      </c>
+        <v>732</v>
+      </c>
+      <c r="N130" s="2"/>
       <c r="O130" s="2"/>
       <c r="P130" t="s" s="2">
         <v>75</v>
@@ -17140,13 +17117,13 @@
         <v>75</v>
       </c>
       <c r="X130" t="s" s="2">
-        <v>164</v>
+        <v>75</v>
       </c>
       <c r="Y130" t="s" s="2">
-        <v>735</v>
+        <v>75</v>
       </c>
       <c r="Z130" t="s" s="2">
-        <v>736</v>
+        <v>75</v>
       </c>
       <c r="AA130" t="s" s="2">
         <v>75</v>
@@ -17164,13 +17141,13 @@
         <v>75</v>
       </c>
       <c r="AF130" t="s" s="2">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="AG130" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH130" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="AI130" t="s" s="2">
         <v>98</v>
@@ -17182,7 +17159,7 @@
         <v>75</v>
       </c>
       <c r="AL130" t="s" s="2">
-        <v>728</v>
+        <v>721</v>
       </c>
       <c r="AM130" t="s" s="2">
         <v>75</v>
@@ -17190,10 +17167,10 @@
     </row>
     <row r="131" hidden="true">
       <c r="A131" t="s" s="2">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="B131" t="s" s="2">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="C131" s="2"/>
       <c r="D131" t="s" s="2">
@@ -17216,13 +17193,13 @@
         <v>75</v>
       </c>
       <c r="K131" t="s" s="2">
-        <v>320</v>
+        <v>734</v>
       </c>
       <c r="L131" t="s" s="2">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="M131" t="s" s="2">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="N131" s="2"/>
       <c r="O131" s="2"/>
@@ -17273,7 +17250,7 @@
         <v>75</v>
       </c>
       <c r="AF131" t="s" s="2">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="AG131" t="s" s="2">
         <v>76</v>
@@ -17291,7 +17268,7 @@
         <v>75</v>
       </c>
       <c r="AL131" t="s" s="2">
-        <v>728</v>
+        <v>721</v>
       </c>
       <c r="AM131" t="s" s="2">
         <v>75</v>
@@ -17299,10 +17276,10 @@
     </row>
     <row r="132" hidden="true">
       <c r="A132" t="s" s="2">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="B132" t="s" s="2">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="C132" s="2"/>
       <c r="D132" t="s" s="2">
@@ -17325,13 +17302,13 @@
         <v>75</v>
       </c>
       <c r="K132" t="s" s="2">
-        <v>741</v>
+        <v>734</v>
       </c>
       <c r="L132" t="s" s="2">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="M132" t="s" s="2">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="N132" s="2"/>
       <c r="O132" s="2"/>
@@ -17382,7 +17359,7 @@
         <v>75</v>
       </c>
       <c r="AF132" t="s" s="2">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="AG132" t="s" s="2">
         <v>76</v>
@@ -17400,7 +17377,7 @@
         <v>75</v>
       </c>
       <c r="AL132" t="s" s="2">
-        <v>728</v>
+        <v>721</v>
       </c>
       <c r="AM132" t="s" s="2">
         <v>75</v>
@@ -17408,10 +17385,10 @@
     </row>
     <row r="133" hidden="true">
       <c r="A133" t="s" s="2">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="B133" t="s" s="2">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="C133" s="2"/>
       <c r="D133" t="s" s="2">
@@ -17434,15 +17411,17 @@
         <v>75</v>
       </c>
       <c r="K133" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="L133" t="s" s="2">
         <v>741</v>
       </c>
-      <c r="L133" t="s" s="2">
-        <v>745</v>
-      </c>
       <c r="M133" t="s" s="2">
-        <v>746</v>
-      </c>
-      <c r="N133" s="2"/>
+        <v>742</v>
+      </c>
+      <c r="N133" t="s" s="2">
+        <v>306</v>
+      </c>
       <c r="O133" s="2"/>
       <c r="P133" t="s" s="2">
         <v>75</v>
@@ -17491,7 +17470,7 @@
         <v>75</v>
       </c>
       <c r="AF133" t="s" s="2">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="AG133" t="s" s="2">
         <v>76</v>
@@ -17509,7 +17488,7 @@
         <v>75</v>
       </c>
       <c r="AL133" t="s" s="2">
-        <v>728</v>
+        <v>107</v>
       </c>
       <c r="AM133" t="s" s="2">
         <v>75</v>
@@ -17517,10 +17496,10 @@
     </row>
     <row r="134" hidden="true">
       <c r="A134" t="s" s="2">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="B134" t="s" s="2">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="C134" s="2"/>
       <c r="D134" t="s" s="2">
@@ -17531,7 +17510,7 @@
         <v>76</v>
       </c>
       <c r="G134" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H134" t="s" s="2">
         <v>75</v>
@@ -17543,18 +17522,20 @@
         <v>75</v>
       </c>
       <c r="K134" t="s" s="2">
-        <v>103</v>
+        <v>744</v>
       </c>
       <c r="L134" t="s" s="2">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="M134" t="s" s="2">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="N134" t="s" s="2">
-        <v>306</v>
-      </c>
-      <c r="O134" s="2"/>
+        <v>714</v>
+      </c>
+      <c r="O134" t="s" s="2">
+        <v>747</v>
+      </c>
       <c r="P134" t="s" s="2">
         <v>75</v>
       </c>
@@ -17602,145 +17583,32 @@
         <v>75</v>
       </c>
       <c r="AF134" t="s" s="2">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="AG134" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH134" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AI134" t="s" s="2">
         <v>98</v>
       </c>
       <c r="AJ134" t="s" s="2">
-        <v>99</v>
+        <v>368</v>
       </c>
       <c r="AK134" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AL134" t="s" s="2">
-        <v>107</v>
+        <v>748</v>
       </c>
       <c r="AM134" t="s" s="2">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="135" hidden="true">
-      <c r="A135" t="s" s="2">
-        <v>750</v>
-      </c>
-      <c r="B135" t="s" s="2">
-        <v>750</v>
-      </c>
-      <c r="C135" s="2"/>
-      <c r="D135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="E135" s="2"/>
-      <c r="F135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="G135" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="H135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="I135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="J135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="K135" t="s" s="2">
-        <v>751</v>
-      </c>
-      <c r="L135" t="s" s="2">
-        <v>752</v>
-      </c>
-      <c r="M135" t="s" s="2">
-        <v>753</v>
-      </c>
-      <c r="N135" t="s" s="2">
-        <v>721</v>
-      </c>
-      <c r="O135" t="s" s="2">
-        <v>754</v>
-      </c>
-      <c r="P135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="Q135" s="2"/>
-      <c r="R135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="S135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="T135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="U135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="V135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="W135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="X135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="Y135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="Z135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AA135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AB135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AC135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AD135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AE135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AF135" t="s" s="2">
-        <v>750</v>
-      </c>
-      <c r="AG135" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AH135" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AI135" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AJ135" t="s" s="2">
-        <v>368</v>
-      </c>
-      <c r="AK135" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AL135" t="s" s="2">
-        <v>755</v>
-      </c>
-      <c r="AM135" t="s" s="2">
         <v>75</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM135">
+  <autoFilter ref="A1:AM134">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -17750,7 +17618,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI134">
+  <conditionalFormatting sqref="A2:AI133">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>